<commit_message>
Updated debugging scripts for water consumption
</commit_message>
<xml_diff>
--- a/debugging/results/export_TEMBA_ENB_ref/Mixes_percentages_TEMBA_ENB_ref.xlsx
+++ b/debugging/results/export_TEMBA_ENB_ref/Mixes_percentages_TEMBA_ENB_ref.xlsx
@@ -30,8 +30,8 @@
     <sheet name="Max values_hydro" sheetId="21" state="visible" r:id="rId21"/>
     <sheet name="Max values_fpv" sheetId="22" state="visible" r:id="rId22"/>
     <sheet name="TotalWaterConsumption" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="Water Consumption (No Hydro)" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="Water Consumption (Detail Hydro)" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="WaterConsumption(No Hydro)" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="WaterConsumption(Detail Hydro)" sheetId="25" state="visible" r:id="rId25"/>
     <sheet name="Total Costs" sheetId="26" state="visible" r:id="rId26"/>
   </sheets>
   <definedNames/>
@@ -32327,8 +32327,12 @@
       <c r="H2" t="n">
         <v>2070</v>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+      <c r="I2" t="n">
+        <v>0.02754190943981545</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2070</v>
+      </c>
       <c r="K2" t="n">
         <v>2027</v>
       </c>
@@ -32514,7 +32518,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Water Consumption (No Hydro)</t>
+          <t>WaterConsumption(No Hydro)</t>
         </is>
       </c>
     </row>
@@ -32545,7 +32549,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Water Consumption (Detail Hydro)</t>
+          <t>WaterConsumption(Detail Hydro)</t>
         </is>
       </c>
     </row>

</xml_diff>